<commit_message>
New Spell structuring completed
</commit_message>
<xml_diff>
--- a/CoreRulebook/Data/Spells/recuperation.xlsx
+++ b/CoreRulebook/Data/Spells/recuperation.xlsx
@@ -20,11 +20,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="176">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
   <si>
+    <t xml:space="preserve">Discipline</t>
+  </si>
+  <si>
     <t xml:space="preserve">Incantation</t>
   </si>
   <si>
@@ -40,18 +43,6 @@
     <t xml:space="preserve">Level</t>
   </si>
   <si>
-    <t xml:space="preserve">Fortitude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attribute</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proficiency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Difficulty</t>
-  </si>
-  <si>
     <t xml:space="preserve">Resist</t>
   </si>
   <si>
@@ -67,6 +58,9 @@
     <t xml:space="preserve">Aid Charm</t>
   </si>
   <si>
+    <t xml:space="preserve">Healing</t>
+  </si>
+  <si>
     <t xml:space="preserve">subsidium</t>
   </si>
   <si>
@@ -79,9 +73,6 @@
     <t xml:space="preserve">1 hour</t>
   </si>
   <si>
-    <t xml:space="preserve">EMP </t>
-  </si>
-  <si>
     <t xml:space="preserve">Raise the HP ceiling of a target by 3. If target has HP$&gt;0$, also increase HP by this amount.</t>
   </si>
   <si>
@@ -175,6 +166,9 @@
     <t xml:space="preserve">Caterwauling Ward</t>
   </si>
   <si>
+    <t xml:space="preserve">Warding</t>
+  </si>
+  <si>
     <t xml:space="preserve">caterwaul</t>
   </si>
   <si>
@@ -182,9 +176,6 @@
   </si>
   <si>
     <t xml:space="preserve">2 weeks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INT</t>
   </si>
   <si>
     <t xml:space="preserve">FIN(Stealth)</t>
@@ -206,9 +197,6 @@
     <t xml:space="preserve">Etheral Shield</t>
   </si>
   <si>
-    <t xml:space="preserve">POW</t>
-  </si>
-  <si>
     <t xml:space="preserve">Erects an ethereal shield in front of you that absorbs incoming magical attacks.
 Shielding charm provides a magical AC by 10+PP against all incoming spells, but does not protect against physical damage, or the aftereffects of magic (i.e. a nearby explosion). This AC is eroded by all damage-causing effects.</t>
   </si>
@@ -252,12 +240,6 @@
     <t xml:space="preserve">Yellow-white rays</t>
   </si>
   <si>
-    <t xml:space="preserve">EMP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Healing</t>
-  </si>
-  <si>
     <t xml:space="preserve">Heal for 2 points per turn. 
 If the target has a serious wound, i.e. a broken bone, cannot heal beyond 50\% health. Only works on living creatures. </t>
   </si>
@@ -268,9 +250,6 @@
     <t xml:space="preserve">muffliato</t>
   </si>
   <si>
-    <t xml:space="preserve">SPR</t>
-  </si>
-  <si>
     <t xml:space="preserve">A buzzing sound fills the ears of anyone trying to listen in on your conversations whilst you are in the warded area. Lasts for one hour, and has a radius of 2m.</t>
   </si>
   <si>
@@ -283,9 +262,6 @@
     <t xml:space="preserve">Brick-red rays</t>
   </si>
   <si>
-    <t xml:space="preserve">Arcane</t>
-  </si>
-  <si>
     <t xml:space="preserve">Restore the strength of a target shield or magical ward by (2+PP) points per turn that this spell is maintained. Cannot restore the strength to more than the original level.</t>
   </si>
   <si>
@@ -304,9 +280,6 @@
     <t xml:space="preserve">5 minutes</t>
   </si>
   <si>
-    <t xml:space="preserve">Endurance</t>
-  </si>
-  <si>
     <t xml:space="preserve">Increase the target{\apos} AC by 10+PP. </t>
   </si>
   <si>
@@ -377,9 +350,6 @@
     <t xml:space="preserve">dispungo</t>
   </si>
   <si>
-    <t xml:space="preserve">Understand Other</t>
-  </si>
-  <si>
     <t xml:space="preserve">Enquire as to the health status of the target, find out their remaining HP, as well as any status effects they currently posses. </t>
   </si>
   <si>
@@ -476,13 +446,10 @@
     <t xml:space="preserve">White flash</t>
   </si>
   <si>
-    <t xml:space="preserve">Willpower</t>
-  </si>
-  <si>
     <t xml:space="preserve">ATH (Strength)</t>
   </si>
   <si>
-    <t xml:space="preserve">Force objects and beings to release the target from their grip if they fail a Resist check. </t>
+    <t xml:space="preserve">Force objects and beings to release the target , and remove all impediments to moving. Resist nullifies this effect.</t>
   </si>
   <si>
     <t xml:space="preserve">Runic Shield</t>
@@ -624,9 +591,6 @@
     <t xml:space="preserve">denarlium</t>
   </si>
   <si>
-    <t xml:space="preserve">Precision</t>
-  </si>
-  <si>
     <t xml:space="preserve">ATH (Perception)</t>
   </si>
   <si>
@@ -712,9 +676,6 @@
   </si>
   <si>
     <t xml:space="preserve">5 days</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stealth</t>
   </si>
   <si>
     <t xml:space="preserve">A ward that creates an invisible trap of 2m in radius. When a being crosses over the threshold, the ward slams shut, doing 2d8 worth of piercing damage and applying the Trapped status effect. </t>
@@ -751,9 +712,6 @@
     <t xml:space="preserve">3 + PP minutes</t>
   </si>
   <si>
-    <t xml:space="preserve">FIN </t>
-  </si>
-  <si>
     <t xml:space="preserve">This spell creates a permanent warded area inside which all magic performs exactly the opposite to its intended purpose. Healing spells cause harm, hexes heal and shields amplify the spells passing through them. </t>
   </si>
   <si>
@@ -857,9 +815,6 @@
     <t xml:space="preserve">Invisible ripple</t>
   </si>
   <si>
-    <t xml:space="preserve">Strength</t>
-  </si>
-  <si>
     <t xml:space="preserve">Erects a 1m radius shield in front of the caster, which halts any physical object that touches it. Objects in flight drop to the ground, as if the {\it Halt} spell had been cast on them.</t>
   </si>
   <si>
@@ -870,6 +825,45 @@
   </si>
   <si>
     <t xml:space="preserve">Target is protected from the ravages of the environment, and hence can exist in temperatures in the range -40  to 50 celsius, and is unaffected by heavy rain and other weather phenomena. Does not protect against heat damage. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patronus Charm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expecto patronus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Summon your greatest, happiest memories into physical form: your patronus. The patronus will prevent any Un-Life creatures from approaching you for the duration of the spell.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="aakar"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">When cast by a character higher than 15</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="8"/>
+        <rFont val="aakar"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="aakar"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> level, the patronus takes corporeal form, and may attack Unlife directly, doing 5d8 Holy damage.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -879,7 +873,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -918,6 +912,12 @@
       <sz val="8"/>
       <name val="aakar"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -963,7 +963,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -984,6 +984,14 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -997,22 +1005,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:M36" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:M36"/>
-  <tableColumns count="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J36" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:J36"/>
+  <tableColumns count="10">
     <tableColumn id="1" name="Name"/>
-    <tableColumn id="2" name="Incantation"/>
-    <tableColumn id="3" name="Type"/>
-    <tableColumn id="4" name="TravelType"/>
-    <tableColumn id="5" name="Duration"/>
-    <tableColumn id="6" name="Level"/>
-    <tableColumn id="7" name="Fortitude"/>
-    <tableColumn id="8" name="Attribute"/>
-    <tableColumn id="9" name="Proficiency"/>
-    <tableColumn id="10" name="Difficulty"/>
-    <tableColumn id="11" name="Resist"/>
-    <tableColumn id="12" name="ResistDV"/>
-    <tableColumn id="13" name="Effect"/>
+    <tableColumn id="2" name="Discipline"/>
+    <tableColumn id="3" name="Incantation"/>
+    <tableColumn id="4" name="Type"/>
+    <tableColumn id="5" name="TravelType"/>
+    <tableColumn id="6" name="Duration"/>
+    <tableColumn id="7" name="Level"/>
+    <tableColumn id="8" name="Resist"/>
+    <tableColumn id="9" name="ResistDV"/>
+    <tableColumn id="10" name="Effect"/>
   </tableColumns>
 </table>
 </file>
@@ -1022,26 +1027,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I5" activeCellId="0" sqref="I5"/>
+      <selection pane="bottomRight" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="36.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="5" style="1" width="8.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="72.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="29.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="1" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="36.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="72.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="29.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="12" style="1" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1021" style="0" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1072,1364 +1078,1090 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="G2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="F2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="G3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
+      <c r="I3" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="F3" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3" s="3" t="n">
-        <v>15</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="F4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="K4" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="26.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="F5" s="3" t="n">
+      <c r="G5" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="G5" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="4" t="s">
-        <v>41</v>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="3" t="n">
+        <v>37</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="G6" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="4" t="s">
-        <v>45</v>
+      <c r="J6" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="F7" s="3" t="n">
+      <c r="G7" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="G7" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J7" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>51</v>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" s="3" t="n">
+        <v>46</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="G8" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="J8" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="4" t="s">
-        <v>57</v>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="F9" s="3" t="n">
+      <c r="G9" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="G9" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="H9" s="3"/>
       <c r="I9" s="3"/>
-      <c r="J9" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>62</v>
+      <c r="J9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3" t="n">
+        <v>55</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="F10" s="3" t="n">
+      <c r="G10" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="G10" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J10" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="4" t="s">
-        <v>66</v>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E11" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="F11" s="3" t="n">
+      <c r="G11" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="G11" s="3" t="n">
-        <v>5</v>
-      </c>
       <c r="H11" s="3" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J11" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>72</v>
+        <v>61</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="F12" s="3" t="n">
+      <c r="G12" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="G12" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J12" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>76</v>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>78</v>
+        <v>20</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F13" s="3" t="n">
+        <v>68</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="G13" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="H13" s="3"/>
       <c r="I13" s="3"/>
-      <c r="J13" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>81</v>
+      <c r="J13" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>83</v>
+        <v>20</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F14" s="3" t="n">
+        <v>73</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="G14" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="H14" s="3"/>
       <c r="I14" s="3"/>
-      <c r="J14" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="4" t="s">
-        <v>85</v>
+      <c r="J14" s="4" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E15" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" s="3" t="n">
+      <c r="G16" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="G15" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="J15" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="M15" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="G16" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J16" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="4" t="s">
-        <v>95</v>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="4" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>97</v>
+        <v>12</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="F17" s="3" t="n">
+      <c r="G17" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="G17" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J17" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="4" t="s">
-        <v>98</v>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="4" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F18" s="3" t="n">
+        <v>89</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G18" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="G18" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="H18" s="3"/>
       <c r="I18" s="3"/>
-      <c r="J18" s="3" t="n">
-        <v>9</v>
-      </c>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="4" t="s">
-        <v>102</v>
+      <c r="J18" s="4" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>104</v>
+        <v>20</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="F19" s="3" t="n">
+        <v>93</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G19" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="G19" s="3" t="n">
-        <v>8</v>
-      </c>
       <c r="H19" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J19" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="L19" s="3" t="n">
+        <v>95</v>
+      </c>
+      <c r="I19" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="M19" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="N19" s="2" t="s">
-        <v>108</v>
+      <c r="J19" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="26.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>110</v>
+        <v>12</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>111</v>
+        <v>14</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="F20" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G20" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="G20" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J20" s="3" t="n">
-        <v>9</v>
-      </c>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="4" t="s">
-        <v>113</v>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>115</v>
+        <v>20</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F21" s="3" t="n">
+        <v>104</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G21" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="G21" s="3" t="n">
-        <v>16</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="H21" s="3"/>
       <c r="I21" s="3"/>
-      <c r="J21" s="3" t="n">
-        <v>9</v>
-      </c>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="4" t="s">
-        <v>116</v>
+      <c r="J21" s="4" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>118</v>
+        <v>12</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>16</v>
+        <v>107</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="F22" s="3" t="n">
+      <c r="G22" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="G22" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J22" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="N22" s="2" t="s">
-        <v>120</v>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>122</v>
+        <v>20</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F23" s="3" t="n">
+        <v>111</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G23" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="G23" s="3" t="n">
-        <v>12</v>
-      </c>
       <c r="H23" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="J23" s="3" t="n">
+        <v>112</v>
+      </c>
+      <c r="I23" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="K23" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="L23" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="M23" s="4" t="s">
-        <v>125</v>
+      <c r="J23" s="4" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="26.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>31</v>
+        <v>115</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="F24" s="3" t="n">
+      <c r="G24" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="G24" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="H24" s="3"/>
       <c r="I24" s="3"/>
-      <c r="J24" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="4" t="s">
-        <v>128</v>
+      <c r="J24" s="4" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>130</v>
+        <v>12</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F25" s="3" t="n">
+        <v>118</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G25" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="G25" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="H25" s="3"/>
       <c r="I25" s="3"/>
-      <c r="J25" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="29.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J25" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>133</v>
+        <v>20</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="F26" s="3" t="n">
+        <v>121</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="G26" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="G26" s="3" t="n">
-        <v>9</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="H26" s="3"/>
       <c r="I26" s="3"/>
-      <c r="J26" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="N26" s="2" t="s">
-        <v>136</v>
+      <c r="J26" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>138</v>
+        <v>20</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="F27" s="3" t="n">
+        <v>126</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="G27" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="G27" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="H27" s="3"/>
       <c r="I27" s="3"/>
-      <c r="J27" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="4" t="s">
-        <v>140</v>
+      <c r="J27" s="4" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>142</v>
+        <v>20</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="F28" s="3" t="n">
+        <v>130</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G28" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="G28" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="J28" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="N28" s="2" t="s">
-        <v>108</v>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>147</v>
+        <v>12</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>16</v>
+        <v>134</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="F29" s="3" t="n">
+        <v>34</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="G29" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="G29" s="3" t="n">
-        <v>11</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J29" s="3" t="n">
-        <v>9</v>
-      </c>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="4" t="s">
-        <v>149</v>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="4" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="26.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>151</v>
+        <v>20</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3" t="n">
+        <v>138</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="F30" s="3" t="n">
+      <c r="G30" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="G30" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="H30" s="3"/>
       <c r="I30" s="3"/>
-      <c r="J30" s="3" t="n">
-        <v>11</v>
-      </c>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="4" t="s">
-        <v>152</v>
+      <c r="J30" s="4" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>154</v>
+        <v>20</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="F31" s="3" t="n">
+        <v>141</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="G31" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="G31" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>156</v>
-      </c>
+      <c r="H31" s="3"/>
       <c r="I31" s="3"/>
-      <c r="J31" s="3" t="n">
-        <v>11</v>
-      </c>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="4" t="s">
-        <v>157</v>
+      <c r="J31" s="4" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>159</v>
+        <v>20</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="F32" s="3" t="n">
+        <v>145</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G32" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="G32" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="H32" s="3"/>
       <c r="I32" s="3"/>
-      <c r="J32" s="3" t="n">
-        <v>9</v>
-      </c>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="N32" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J32" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>164</v>
+        <v>12</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>16</v>
+        <v>150</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E33" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F33" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="F33" s="3" t="n">
+      <c r="G33" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="G33" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J33" s="3" t="n">
-        <v>9</v>
-      </c>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="4" t="s">
-        <v>165</v>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="4" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="42.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>167</v>
+        <v>20</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3" t="n">
+        <v>153</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="F34" s="3" t="n">
+      <c r="G34" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="G34" s="3" t="n">
-        <v>20</v>
-      </c>
       <c r="H34" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3" t="n">
+        <v>155</v>
+      </c>
+      <c r="I34" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="K34" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="L34" s="3" t="n">
-        <v>18</v>
-      </c>
-      <c r="M34" s="4" t="s">
-        <v>170</v>
+      <c r="J34" s="4" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>172</v>
+        <v>20</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F35" s="3" t="n">
+        <v>158</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G35" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="G35" s="3" t="n">
-        <v>18</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="H35" s="3"/>
       <c r="I35" s="3"/>
-      <c r="J35" s="3" t="n">
-        <v>14</v>
-      </c>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="4" t="s">
-        <v>173</v>
+      <c r="J35" s="4" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>175</v>
+        <v>12</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="E36" s="3" t="n">
+        <v>162</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="F36" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="F36" s="3" t="n">
+      <c r="G36" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="G36" s="3" t="n">
-        <v>20</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J36" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-      <c r="M36" s="4" t="s">
-        <v>178</v>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="4" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>180</v>
+        <v>20</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>31</v>
+        <v>166</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E37" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F37" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F37" s="1" t="n">
+      <c r="G37" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G37" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="J37" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="M37" s="2" t="s">
-        <v>183</v>
+      <c r="J37" s="2" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>185</v>
+        <v>12</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F38" s="1" t="n">
+        <v>170</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G38" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="G38" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J38" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="M38" s="2" t="s">
-        <v>186</v>
+      <c r="J38" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>